<commit_message>
Doc updates. stop tracking Doc Source/Build directory
</commit_message>
<xml_diff>
--- a/Documentation Source/source/electronics bom.xlsx
+++ b/Documentation Source/source/electronics bom.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Repos/Syringe/Documentation Source/source/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Repos/karpova_lab/Syringe/Documentation Source/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -191,6 +191,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -512,7 +513,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -758,7 +759,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Update documentation and frame CAD
</commit_message>
<xml_diff>
--- a/Documentation Source/source/electronics bom.xlsx
+++ b/Documentation Source/source/electronics bom.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Repos/karpova_lab/Syringe/Documentation Source/source/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/Syringe/Documentation Source/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="4800" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>link</t>
   </si>
@@ -62,9 +62,6 @@
     <t>0.1" breakaway header</t>
   </si>
   <si>
-    <t>Reed Switch</t>
-  </si>
-  <si>
     <t>Motor Driver</t>
   </si>
   <si>
@@ -86,15 +83,6 @@
     <t>http://www.digikey.com/product-detail/en/microchip-technology/ATMEGA328P-ANR/ATMEGA328P-ANRCT-ND/2774230</t>
   </si>
   <si>
-    <t>Magnet</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/radial-magnet-inc/8177/469-1051-ND/5400490</t>
-  </si>
-  <si>
-    <t>MK04-1A66B-500W</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/products/en?x=0&amp;y=0&amp;lang=en&amp;site=us&amp;keywords=PCE3961CT-ND</t>
   </si>
   <si>
@@ -146,16 +134,16 @@
     <t>Vertical RJ45</t>
   </si>
   <si>
-    <t>https://www.digikey.com/products/en?keywords=374-1115-nd</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/molex-llc/0901200132/WM8082-ND/760797</t>
+  </si>
+  <si>
+    <t>3.3v dc regulator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -242,6 +230,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -509,11 +500,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -562,31 +553,28 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C2" s="1">
-        <v>14.95</v>
+        <v>2.25</v>
       </c>
       <c r="D2" s="1" t="str">
         <f>CONCATENATE("`",F2," &lt;",G2,"&gt;`_")</f>
-        <v>`2900 &lt;http://www.digikey.com/products/en?x=0&amp;y=0&amp;lang=en&amp;site=us&amp;keywords=1528-1547-ND&gt;`_</v>
-      </c>
-      <c r="E2" s="1" t="s">
+        <v>`ATMEGA328P &lt;http://www.digikey.com/product-detail/en/microchip-technology/ATMEGA328P-ANR/ATMEGA328P-ANRCT-ND/2774230&gt;`_</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1">
-        <v>2900</v>
-      </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1">
         <v>1</v>
       </c>
       <c r="I2" s="1">
         <f>C2/H2</f>
-        <v>14.95</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -594,27 +582,27 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1">
-        <v>1.45</v>
+        <v>3.33</v>
       </c>
       <c r="D3" s="1" t="str">
         <f>CONCATENATE("`",F3," &lt;",G3,"&gt;`_")</f>
-        <v>`901200132 &lt;https://www.digikey.com/product-detail/en/molex-llc/0901200132/WM8082-ND/760797&gt;`_</v>
-      </c>
-      <c r="F3" s="5">
-        <v>901200132</v>
+        <v>`A3967SLBT &lt;http://www.digikey.com/product-detail/en/allegro-microsystems-llc/A3967SLBTR-T/620-1140-1-ND/1090383&gt;`_</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I12" si="0">C3/H3</f>
-        <v>1.45</v>
+        <f>C3/H3</f>
+        <v>3.33</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -622,254 +610,206 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1">
-        <v>1.49</v>
+        <v>14.95</v>
       </c>
       <c r="D4" s="1" t="str">
         <f>CONCATENATE("`",F4," &lt;",G4,"&gt;`_")</f>
+        <v>`2900 &lt;http://www.digikey.com/products/en?x=0&amp;y=0&amp;lang=en&amp;site=us&amp;keywords=1528-1547-ND&gt;`_</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2900</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <f>C4/H4</f>
+        <v>14.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f>CONCATENATE("`",F5," &lt;",G5,"&gt;`_")</f>
+        <v>`901200132 &lt;https://www.digikey.com/product-detail/en/molex-llc/0901200132/WM8082-ND/760797&gt;`_</v>
+      </c>
+      <c r="F5" s="5">
+        <v>901200132</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" ref="I5:I10" si="0">C5/H5</f>
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.49</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f>CONCATENATE("`",F6," &lt;",G6,"&gt;`_")</f>
         <v>`216550-1 &lt;https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/216550-1/A99308CT-ND/1920159&gt;`_</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1">
+      <c r="F6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
         <f t="shared" si="0"/>
         <v>1.49</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2.13</v>
-      </c>
-      <c r="D5" s="1" t="str">
-        <f>CONCATENATE("`",F5," &lt;",G5,"&gt;`_")</f>
-        <v>`MK04-1A66B-500W &lt;https://www.digikey.com/products/en?keywords=374-1115-nd&gt;`_</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1">
-        <f t="shared" si="0"/>
-        <v>2.13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2.25</v>
-      </c>
-      <c r="D6" s="1" t="str">
-        <f>CONCATENATE("`",F6," &lt;",G6,"&gt;`_")</f>
-        <v>`ATMEGA328P &lt;http://www.digikey.com/product-detail/en/microchip-technology/ATMEGA328P-ANR/ATMEGA328P-ANRCT-ND/2774230&gt;`_</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1">
-        <f t="shared" si="0"/>
-        <v>2.25</v>
-      </c>
-    </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1">
-        <v>3.33</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1" t="str">
-        <f t="shared" ref="D7:D9" si="1">CONCATENATE("`",F7," &lt;",G7,"&gt;`_")</f>
-        <v>`A3967SLBT &lt;http://www.digikey.com/product-detail/en/allegro-microsystems-llc/A3967SLBTR-T/620-1140-1-ND/1090383&gt;`_</v>
+        <f t="shared" ref="D7" si="1">CONCATENATE("`",F7," &lt;",G7,"&gt;`_")</f>
+        <v>`EEE-1VA470WP &lt;http://www.digikey.com/products/en?x=0&amp;y=0&amp;lang=en&amp;site=us&amp;keywords=PCE3961CT-ND&gt;`_</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H7" s="1">
         <v>1</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="0"/>
-        <v>3.33</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
-        <v>1</v>
+      <c r="A8" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1">
-        <v>0.96</v>
+        <v>4.53</v>
       </c>
       <c r="D8" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>`8177 &lt;http://www.digikey.com/product-detail/en/radial-magnet-inc/8177/469-1051-ND/5400490&gt;`_</v>
-      </c>
-      <c r="F8" s="1">
-        <v>8177</v>
+        <f t="shared" ref="D8:D9" si="2">CONCATENATE("`",F8," &lt;",G8,"&gt;`_")</f>
+        <v>`XN2A-1470 &lt;https://www.digikey.com/products/en/connectors-interconnects/rectangular-connectors-free-hanging-panel-mount/316?k=OR1021&gt;`_</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="H8" s="1">
         <v>1</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
-        <v>0.96</v>
+        <v>4.53</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
-        <v>1</v>
+      <c r="A9" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1">
-        <v>1</v>
+        <v>2.95</v>
       </c>
       <c r="D9" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>`EEE-1VA470WP &lt;http://www.digikey.com/products/en?x=0&amp;y=0&amp;lang=en&amp;site=us&amp;keywords=PCE3961CT-ND&gt;`_</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>23</v>
+        <f t="shared" si="2"/>
+        <v>`XN2D-1471 &lt;https://www.digikey.com/product-detail/en/omron-electronics-inc-emc-div/XN2D-1471/OR1027-ND/2330565&gt;`_</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H9" s="1">
         <v>1</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>29</v>
+      <c r="A10" s="4">
+        <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1">
-        <v>4.53</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1" t="str">
-        <f t="shared" ref="D10:D11" si="2">CONCATENATE("`",F10," &lt;",G10,"&gt;`_")</f>
-        <v>`XN2A-1470 &lt;https://www.digikey.com/products/en/connectors-interconnects/rectangular-connectors-free-hanging-panel-mount/316?k=OR1021&gt;`_</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>32</v>
+        <f>CONCATENATE("`",F10," &lt;",G10,"&gt;`_")</f>
+        <v>`972 &lt;https://www.pololu.com/product/972/&gt;`_</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1">
+        <v>972</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="H10" s="1">
         <v>1</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="0"/>
-        <v>4.53</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="1">
-        <v>2.95</v>
-      </c>
-      <c r="D11" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>`XN2D-1471 &lt;https://www.digikey.com/product-detail/en/omron-electronics-inc-emc-div/XN2D-1471/OR1027-ND/2330565&gt;`_</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="I11" s="1">
-        <f t="shared" si="0"/>
-        <v>2.95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
-        <v>1</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="str">
-        <f>CONCATENATE("`",F12," &lt;",G12,"&gt;`_")</f>
-        <v>`972 &lt;https://www.pololu.com/product/972/&gt;`_</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="1">
-        <v>972</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1</v>
-      </c>
-      <c r="I12" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>